<commit_message>
implemented new input template supporting data needed for rapid drawdown
</commit_message>
<xml_diff>
--- a/docs/input_template_dam2.xlsx
+++ b/docs/input_template_dam2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBDD3D3-0CA3-F64F-9552-84D7F425701A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D382347-AE70-1D48-98F0-357E76128C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="1600" windowWidth="38440" windowHeight="24340" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="2280" yWindow="1840" windowWidth="32920" windowHeight="24340" activeTab="4" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,11 @@
   </sheets>
   <definedNames>
     <definedName name="core">profile!$B$5</definedName>
-    <definedName name="crack_depth">main!$D$17</definedName>
-    <definedName name="crack_depth_water">main!$D$18</definedName>
+    <definedName name="crack_depth">main!$D$19</definedName>
+    <definedName name="crack_depth_water">main!$D$20</definedName>
     <definedName name="crest">profile!$B$4</definedName>
-    <definedName name="gamma_w">main!$D$16</definedName>
-    <definedName name="k">main!$D$19</definedName>
+    <definedName name="gamma_w">main!$D$18</definedName>
+    <definedName name="k">main!$D$21</definedName>
     <definedName name="max_depth">circles!$C$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="126">
   <si>
     <t>X</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>FT = Transverse Force (not used)</t>
+  </si>
+  <si>
+    <t>Template version:</t>
+  </si>
+  <si>
+    <t>2025.06.20</t>
   </si>
 </sst>
 </file>
@@ -2214,6 +2220,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2223,6 +2238,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>302</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2286,6 +2310,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2295,6 +2328,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>302</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4423,10 +4465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4448,164 +4490,172 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="16" t="s">
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D7" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="25"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="23"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C16" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="1">
-        <v>62.4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C18" s="15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>62.4</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
       <c r="C19" s="15" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
+      <c r="C20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
+      <c r="C21" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4631,7 +4681,7 @@
   <dimension ref="A2:N36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B7"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5185,7 +5235,7 @@
   <dimension ref="A2:T13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5331,8 +5381,12 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3">
+        <v>300</v>
+      </c>
+      <c r="J5" s="3">
+        <v>20</v>
+      </c>
       <c r="K5" s="3">
         <v>1</v>
       </c>
@@ -5367,8 +5421,12 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>100</v>
+      </c>
+      <c r="J6" s="3">
+        <v>19</v>
+      </c>
       <c r="K6" s="3">
         <v>1</v>
       </c>
@@ -5623,8 +5681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3821B4BC-2D03-B047-9DB8-8ECD257276B0}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5663,8 +5721,12 @@
       <c r="B4" s="3">
         <v>302</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="3">
+        <v>-150</v>
+      </c>
+      <c r="E4" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
@@ -5673,8 +5735,12 @@
       <c r="B5" s="3">
         <v>302</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3">
+        <v>277.5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
@@ -5683,8 +5749,12 @@
       <c r="B6" s="3">
         <v>275</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3">
+        <v>315</v>
+      </c>
+      <c r="E6" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
@@ -5693,8 +5763,12 @@
       <c r="B7" s="3">
         <v>240</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3">
+        <v>343.5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -5703,8 +5777,12 @@
       <c r="B8" s="3">
         <v>227</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3">
+        <v>590</v>
+      </c>
+      <c r="E8" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -5713,8 +5791,12 @@
       <c r="B9" s="3">
         <v>227</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3">
+        <v>740</v>
+      </c>
+      <c r="E9" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -6149,7 +6231,7 @@
   <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6443,12 +6525,24 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="B17" s="3">
+        <v>-150</v>
+      </c>
+      <c r="C17" s="3">
+        <v>227</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4680</v>
+      </c>
+      <c r="F17" s="3">
+        <v>-150</v>
+      </c>
+      <c r="G17" s="3">
+        <v>227</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4680</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -6457,12 +6551,24 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>227</v>
+      </c>
+      <c r="D18" s="3">
+        <v>4680</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>227</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4680</v>
+      </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -6471,12 +6577,24 @@
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="B19" s="3">
+        <v>225</v>
+      </c>
+      <c r="C19" s="3">
+        <v>302</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>225</v>
+      </c>
+      <c r="G19" s="3">
+        <v>302</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>

</xml_diff>

<commit_message>
debugging why line of thrust is wrong with inclined distributed load. no luck.
</commit_message>
<xml_diff>
--- a/docs/input_template_dam2.xlsx
+++ b/docs/input_template_dam2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D382347-AE70-1D48-98F0-357E76128C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486D1672-46E6-0B47-B719-010807AE0ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1840" windowWidth="32920" windowHeight="24340" activeTab="4" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="2280" yWindow="1840" windowWidth="32920" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -843,6 +843,24 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -858,37 +876,19 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -896,6 +896,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -914,13 +921,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2220,15 +2220,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>-150</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>225</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2238,15 +2229,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>302</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2310,15 +2292,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>-150</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>225</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2328,15 +2301,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>302</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4504,10 +4468,10 @@
       <c r="C7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -4516,10 +4480,10 @@
       <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -4528,10 +4492,10 @@
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -4540,10 +4504,10 @@
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
@@ -4552,10 +4516,10 @@
       <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
@@ -4564,10 +4528,10 @@
       <c r="C12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
@@ -4576,10 +4540,10 @@
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="23"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
@@ -4588,10 +4552,10 @@
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
@@ -4600,11 +4564,11 @@
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C18" s="15" t="s">
@@ -4698,26 +4662,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="D2" s="26" t="s">
+      <c r="B2" s="34"/>
+      <c r="D2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="G2" s="26" t="s">
+      <c r="E2" s="34"/>
+      <c r="G2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="J2" s="26" t="s">
+      <c r="H2" s="34"/>
+      <c r="J2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="M2" s="26" t="s">
+      <c r="K2" s="34"/>
+      <c r="M2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="26"/>
+      <c r="N2" s="34"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -4980,26 +4944,26 @@
       <c r="N18" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="D20" s="26" t="s">
+      <c r="B20" s="34"/>
+      <c r="D20" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="G20" s="26" t="s">
+      <c r="E20" s="34"/>
+      <c r="G20" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="26"/>
-      <c r="J20" s="26" t="s">
+      <c r="H20" s="34"/>
+      <c r="J20" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="M20" s="26" t="s">
+      <c r="K20" s="34"/>
+      <c r="M20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="26"/>
+      <c r="N20" s="34"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -5215,16 +5179,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5249,33 +5213,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
       <c r="S2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="30" t="s">
         <v>104</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -5302,28 +5266,28 @@
       <c r="J3" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="Q3" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="S3" s="26" t="s">
         <v>122</v>
       </c>
     </row>
@@ -5635,34 +5599,34 @@
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:J13 G4:H7">
+  <conditionalFormatting sqref="G4:H7 G8:J13">
     <cfRule type="expression" dxfId="5" priority="7">
       <formula>$D4="mc"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I4:J7">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>$D4="cp"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M4:N13">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O13">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$D4="mc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:J7">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="P4:Q7">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8:Q13">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$D8="mc"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4:Q7">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -5681,7 +5645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3821B4BC-2D03-B047-9DB8-8ECD257276B0}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -5691,14 +5655,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="D2" s="38" t="s">
+      <c r="B2" s="36"/>
+      <c r="D2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5853,7 +5817,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="23" t="s">
         <v>107</v>
       </c>
     </row>
@@ -6230,8 +6194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976BB56-7732-404C-B58A-55DA7F8052B3}">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6247,26 +6211,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="F2" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="J2" s="30" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="J2" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="N2" s="30" t="s">
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="N2" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -6465,26 +6429,26 @@
       <c r="P13" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="F15" s="31" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="F15" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="J15" s="31" t="s">
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="J15" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="N15" s="31" t="s">
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="N15" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -6525,24 +6489,12 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="3">
-        <v>-150</v>
-      </c>
-      <c r="C17" s="3">
-        <v>227</v>
-      </c>
-      <c r="D17" s="3">
-        <v>4680</v>
-      </c>
-      <c r="F17" s="3">
-        <v>-150</v>
-      </c>
-      <c r="G17" s="3">
-        <v>227</v>
-      </c>
-      <c r="H17" s="3">
-        <v>4680</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -6551,24 +6503,12 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="3">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>227</v>
-      </c>
-      <c r="D18" s="3">
-        <v>4680</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>227</v>
-      </c>
-      <c r="H18" s="3">
-        <v>4680</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -6577,24 +6517,12 @@
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="3">
-        <v>225</v>
-      </c>
-      <c r="C19" s="3">
-        <v>302</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>225</v>
-      </c>
-      <c r="G19" s="3">
-        <v>302</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -6701,12 +6629,12 @@
       <c r="P26" s="3"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="24" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="25" t="s">
         <v>116</v>
       </c>
     </row>
@@ -6747,30 +6675,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="G2" s="28" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="G2" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="L2" s="28" t="s">
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="L2" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="Q2" s="28" t="s">
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="Q2" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -7009,30 +6937,30 @@
       <c r="T13" s="3"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="G15" s="28" t="s">
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="G15" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="L15" s="28" t="s">
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="L15" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="Q15" s="28" t="s">
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="Q15" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -7265,30 +7193,30 @@
       <c r="T26" s="3"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="G28" s="28" t="s">
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="G28" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="L28" s="28" t="s">
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="L28" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="Q28" s="28" t="s">
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="Q28" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="28"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="40"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">

</xml_diff>

<commit_message>
changed plotting functions to handle multi-stage inputs (dual piezo lines, dual dloads, d-psi in mat table, etc)
</commit_message>
<xml_diff>
--- a/docs/input_template_dam2.xlsx
+++ b/docs/input_template_dam2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486D1672-46E6-0B47-B719-010807AE0ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6D3913-02E3-8A44-9719-AFF1F7624521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1840" windowWidth="32920" windowHeight="24340" activeTab="7" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="20380" yWindow="1840" windowWidth="32920" windowHeight="24340" activeTab="1" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -3292,6 +3292,103 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001F-704D-4E4F-B7C4-BDC51C67D2D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="32"/>
+          <c:order val="32"/>
+          <c:tx>
+            <c:v>Piezometric Line #2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>piezo!$D$4:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>277.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>343.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>740</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>piezo!$E$4:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1382-8A46-87D5-EBD4792CE100}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4629,8 +4726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CEDAD3-D805-AE4D-9F0D-9E80BF51FF21}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5179,16 +5276,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6194,7 +6291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976BB56-7732-404C-B58A-55DA7F8052B3}">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>

</xml_diff>